<commit_message>
06.09. - finally working
End of project - sent to code review
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiKrausz\Documents\GitHub\POC5---Orange\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF4489-3781-430F-8057-0E7AB913B17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A45DB21-5AED-4D4E-A069-382E5107C037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -214,13 +214,81 @@
   </si>
   <si>
     <t>The list of Types of ranks inside each company , types for which we have to find Min Max Med, one at a time.</t>
+  </si>
+  <si>
+    <t>CodeForGraphasTXTPath</t>
+  </si>
+  <si>
+    <t>GraphsFolderPath</t>
+  </si>
+  <si>
+    <t>Path of the txt file containing VBA code for creating charts.</t>
+  </si>
+  <si>
+    <t>Path to the folder where the PDF files should be saved</t>
+  </si>
+  <si>
+    <t>C:\Users\AndreiKrausz\Documents\GitHub\POC5---Orange\Data\Output\PDF_COMPANII</t>
+  </si>
+  <si>
+    <t>Data\Input\vbaCodeForChars.txt</t>
+  </si>
+  <si>
+    <t>ZipFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\AndreiKrausz.zip</t>
+  </si>
+  <si>
+    <t>SharePointURL</t>
+  </si>
+  <si>
+    <t>SharePointLibraryName</t>
+  </si>
+  <si>
+    <t>SharePointNewFolder</t>
+  </si>
+  <si>
+    <t>MailSubject</t>
+  </si>
+  <si>
+    <t>MailAddress</t>
+  </si>
+  <si>
+    <t>Rezultate Orange</t>
+  </si>
+  <si>
+    <t>andrei.krausz@fwfcompany.com</t>
+  </si>
+  <si>
+    <t>devs/'Shared Folder'/KrauszAndrei</t>
+  </si>
+  <si>
+    <t>Documente partajate/devs/'Shared Folder'/KrauszAndrei/Andreikrausz.zip</t>
+  </si>
+  <si>
+    <t>SharePointPathWhereToUpload</t>
+  </si>
+  <si>
+    <t>https://futureworkforcecompany.sharepoint.com/sites/dreamteam/</t>
+  </si>
+  <si>
+    <t>Documente</t>
+  </si>
+  <si>
+    <t>MailBody</t>
+  </si>
+  <si>
+    <t>Buna ziua,
+Atasat gasiti fisierul arhivat generat ce contoine rezultatele POC Orange.
+Mai jos gasiti linkul si path-ul catre fisierul arhivat ce contine rezultatele POC Orange:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -244,6 +312,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,10 +336,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -275,8 +350,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -589,18 +666,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -648,7 +725,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -658,7 +735,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -742,36 +819,112 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1720,12 +1873,14 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B35" r:id="rId1" xr:uid="{C10973EA-4F38-4CF9-B432-9372838D2432}"/>
+    <hyperlink ref="B25" r:id="rId2" xr:uid="{E4F2ADEC-51B9-4682-A3FC-1950A3C095C4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1737,12 +1892,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1779,7 +1934,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1790,7 +1945,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1904,7 +2059,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2900,12 +3055,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>